<commit_message>
entry 4 and start 5
</commit_message>
<xml_diff>
--- a/datascience_diary/data/planets_moons.xlsx
+++ b/datascience_diary/data/planets_moons.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julie.fisher/Documents/learning/machine_learning/experiments/data_sci_storytime/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julie.fisher/Documents/learning/machine_learning/experiments/datascience_diary/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B0E826-CAA2-2B4D-9685-E3FE7FA26A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B231F1-1A30-DD41-A5E1-8446309DE748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{17F23864-C591-48DA-ABD3-CB397D2BC25F}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1492" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="555">
   <si>
     <t>No</t>
   </si>
@@ -2092,11 +2092,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC265B33-381B-4063-A323-2251A4239B5C}">
-  <dimension ref="A1:AK19"/>
+  <dimension ref="A1:AA19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y12" sqref="Y12"/>
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AG22" sqref="AG22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2127,7 +2127,7 @@
     <col min="27" max="27" width="32.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2209,38 +2209,8 @@
       <c r="AA1" t="s">
         <v>536</v>
       </c>
-      <c r="AB1" t="s">
-        <v>443</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>440</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>444</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>445</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>446</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>447</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>441</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2323,38 +2293,8 @@
       <c r="AA2">
         <v>1000</v>
       </c>
-      <c r="AB2">
-        <v>0.22</v>
-      </c>
-      <c r="AC2">
-        <v>0.06</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
-        <v>0</v>
-      </c>
-      <c r="AG2">
-        <v>0</v>
-      </c>
-      <c r="AH2">
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <v>0.42</v>
-      </c>
-      <c r="AJ2">
-        <v>0</v>
-      </c>
-      <c r="AK2">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2437,38 +2377,8 @@
         <f>4.8*10^20</f>
         <v>4.8E+20</v>
       </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-      <c r="AC3">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="AD3">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
-        <v>0.96499999999999997</v>
-      </c>
-      <c r="AH3">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="AI3">
-        <v>0</v>
-      </c>
-      <c r="AJ3">
-        <v>6.9999999999999994E-5</v>
-      </c>
-      <c r="AK3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2551,38 +2461,8 @@
         <f>1.4*10^21</f>
         <v>1.4E+21</v>
       </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0.04</v>
-      </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
-      <c r="AF4">
-        <v>0</v>
-      </c>
-      <c r="AG4">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="AH4">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="AI4">
-        <v>0.20899999999999999</v>
-      </c>
-      <c r="AJ4">
-        <v>9.2999999999999992E-3</v>
-      </c>
-      <c r="AK4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2665,38 +2545,8 @@
       <c r="AA5" s="4">
         <v>100000</v>
       </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-      <c r="AC5">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5">
-        <v>0</v>
-      </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
-      <c r="AG5">
-        <v>0</v>
-      </c>
-      <c r="AH5">
-        <v>0</v>
-      </c>
-      <c r="AI5">
-        <v>0</v>
-      </c>
-      <c r="AJ5">
-        <v>0.7</v>
-      </c>
-      <c r="AK5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2779,38 +2629,8 @@
         <f>2.5*10^16</f>
         <v>2.5E+16</v>
       </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>3.0000000000000001E-5</v>
-      </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
-      <c r="AG6">
-        <v>0.95299999999999996</v>
-      </c>
-      <c r="AH6">
-        <v>2.7E-2</v>
-      </c>
-      <c r="AI6">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="AJ6">
-        <v>1.6E-2</v>
-      </c>
-      <c r="AK6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2893,38 +2713,8 @@
         <f>1.9*10^27</f>
         <v>1.8999999999999998E+27</v>
       </c>
-      <c r="AB7">
-        <v>0.9</v>
-      </c>
-      <c r="AC7">
-        <v>0.1</v>
-      </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7">
-        <v>2.3999999999999998E-3</v>
-      </c>
-      <c r="AF7">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="AG7">
-        <v>0</v>
-      </c>
-      <c r="AH7">
-        <v>0</v>
-      </c>
-      <c r="AI7">
-        <v>0</v>
-      </c>
-      <c r="AJ7">
-        <v>0</v>
-      </c>
-      <c r="AK7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3007,38 +2797,8 @@
         <f>5.4*10^26</f>
         <v>5.4000000000000007E+26</v>
       </c>
-      <c r="AB8">
-        <v>0.96</v>
-      </c>
-      <c r="AC8">
-        <v>0.04</v>
-      </c>
-      <c r="AD8">
-        <v>0</v>
-      </c>
-      <c r="AE8">
-        <v>2E-3</v>
-      </c>
-      <c r="AF8">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="AG8">
-        <v>0</v>
-      </c>
-      <c r="AH8">
-        <v>0</v>
-      </c>
-      <c r="AI8">
-        <v>0</v>
-      </c>
-      <c r="AJ8">
-        <v>0</v>
-      </c>
-      <c r="AK8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>190</v>
       </c>
@@ -3122,38 +2882,8 @@
         <f>9.1*10^18</f>
         <v>9.1E+18</v>
       </c>
-      <c r="AB9">
-        <v>2E-3</v>
-      </c>
-      <c r="AC9">
-        <v>0</v>
-      </c>
-      <c r="AD9">
-        <v>0</v>
-      </c>
-      <c r="AE9">
-        <v>0.03</v>
-      </c>
-      <c r="AF9">
-        <v>0</v>
-      </c>
-      <c r="AG9">
-        <v>0</v>
-      </c>
-      <c r="AH9">
-        <v>0.82</v>
-      </c>
-      <c r="AI9">
-        <v>0</v>
-      </c>
-      <c r="AJ9">
-        <v>0.12</v>
-      </c>
-      <c r="AK9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3236,38 +2966,8 @@
         <f>8.6*10^25</f>
         <v>8.6E+25</v>
       </c>
-      <c r="AB10">
-        <v>0.85</v>
-      </c>
-      <c r="AC10">
-        <v>0.15</v>
-      </c>
-      <c r="AD10">
-        <v>0</v>
-      </c>
-      <c r="AE10">
-        <v>0</v>
-      </c>
-      <c r="AF10">
-        <v>0</v>
-      </c>
-      <c r="AG10">
-        <v>0</v>
-      </c>
-      <c r="AH10">
-        <v>0</v>
-      </c>
-      <c r="AI10">
-        <v>0</v>
-      </c>
-      <c r="AJ10">
-        <v>0</v>
-      </c>
-      <c r="AK10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3350,38 +3050,8 @@
         <f>1*10^26</f>
         <v>1E+26</v>
       </c>
-      <c r="AB11">
-        <v>0.85</v>
-      </c>
-      <c r="AC11">
-        <v>0.15</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <v>3.0000000000000001E-5</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
-        <v>0</v>
-      </c>
-      <c r="AH11">
-        <v>0</v>
-      </c>
-      <c r="AI11">
-        <v>0</v>
-      </c>
-      <c r="AJ11">
-        <v>0</v>
-      </c>
-      <c r="AK11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3463,36 +3133,6 @@
       <c r="AA12" s="4">
         <f>1.3*10^14</f>
         <v>130000000000000</v>
-      </c>
-      <c r="AB12">
-        <v>0</v>
-      </c>
-      <c r="AC12">
-        <v>0</v>
-      </c>
-      <c r="AD12">
-        <v>0</v>
-      </c>
-      <c r="AE12">
-        <v>0.02</v>
-      </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
-      <c r="AG12">
-        <v>0.08</v>
-      </c>
-      <c r="AH12">
-        <v>0.9</v>
-      </c>
-      <c r="AI12">
-        <v>0</v>
-      </c>
-      <c r="AJ12">
-        <v>0</v>
-      </c>
-      <c r="AK12">
-        <v>0</v>
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>